<commit_message>
Excel data provider coded added.
</commit_message>
<xml_diff>
--- a/input-files/TestData.xlsx
+++ b/input-files/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh\git\repository\SeleniumTraining\input-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8260AB6D-0795-4EC8-BBC7-2258F5740A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A573BB0B-533E-4308-A5F2-485BAFD34822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8629D958-925B-4D14-895A-B49A3E7503E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Testcases</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>zcccfw</t>
-  </si>
-  <si>
-    <t>ssf</t>
   </si>
   <si>
     <t>ff</t>
@@ -450,7 +447,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,11 +504,11 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -519,13 +516,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>